<commit_message>
added charts and photo
</commit_message>
<xml_diff>
--- a/graph.xlsx
+++ b/graph.xlsx
@@ -1,21 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d055b0e410ea8443/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{85EB65EA-CB77-4ADF-B2FB-B27E718AD9BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F0C2919-2018-4526-88CC-FC41A0EEE4C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="2760" windowWidth="28800" windowHeight="15345"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ethanwilkes_colespencer_phw_out" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -49,7 +61,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -626,6 +638,75 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>ethanwilkes_colespencer_phw_out!$O$1:$O$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>105</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>ethanwilkes_colespencer_phw_out!$A$2:$A$20</c:f>
@@ -717,6 +798,75 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>ethanwilkes_colespencer_phw_out!$O$1:$O$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>105</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>ethanwilkes_colespencer_phw_out!$B$2:$B$20</c:f>
@@ -808,6 +958,75 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>ethanwilkes_colespencer_phw_out!$O$1:$O$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>105</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>ethanwilkes_colespencer_phw_out!$C$2:$C$20</c:f>
@@ -899,6 +1118,75 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>ethanwilkes_colespencer_phw_out!$O$1:$O$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>105</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>ethanwilkes_colespencer_phw_out!$D$2:$D$20</c:f>
@@ -969,6 +1257,662 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000005-BEAE-44AE-BC17-E5A639729871}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>N</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>ethanwilkes_colespencer_phw_out!$O$1:$O$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>105</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>ethanwilkes_colespencer_phw_out!$J$1:$J$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>9.9999999999999995E-7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.9999999999999999E-6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0000000000000001E-6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.9999999999999998E-6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.9999999999999996E-6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0000000000000002E-6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.9999999999999999E-6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.9999999999999996E-6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.0000000000000002E-6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9.9999999999999991E-6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.1E-5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.2E-5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.2999999999999999E-5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.4E-5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.4999999999999999E-5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.5999999999999999E-5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.7E-5</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.8E-5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.8999999999999998E-5</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.9999999999999998E-5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000002D-EBC8-44A0-9B7D-9BF9EF3C88C6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>N^2</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>ethanwilkes_colespencer_phw_out!$O$1:$O$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>105</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>ethanwilkes_colespencer_phw_out!$K$1:$K$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.9999999999999999E-12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.0000000000000012E-12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.6E-11</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.4999999999999994E-11</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.6000000000000005E-11</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.8999999999999999E-11</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.3999999999999999E-11</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.1000000000000005E-11</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9.9999999999999978E-11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.21E-10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.4400000000000002E-10</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.6899999999999999E-10</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.96E-10</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.2499999999999997E-10</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.5599999999999999E-10</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.8899999999999998E-10</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.2400000000000002E-10</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3.6099999999999989E-10</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.9999999999999991E-10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000002E-EBC8-44A0-9B7D-9BF9EF3C88C6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:v>N^3</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>ethanwilkes_colespencer_phw_out!$O$1:$O$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>105</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>ethanwilkes_colespencer_phw_out!$L$1:$L$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.999999999999999E-18</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.7000000000000004E-17</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.3999999999999992E-17</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.2499999999999996E-16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.1600000000000003E-16</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.43E-16</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.1199999999999994E-16</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.2900000000000001E-16</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9.9999999999999968E-16</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.3309999999999999E-15</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.7280000000000003E-15</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.1969999999999996E-15</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.744E-15</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.3749999999999994E-15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4.0959999999999995E-15</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4.913E-15</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5.8320000000000001E-15</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>6.8589999999999973E-15</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>7.9999999999999975E-15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000002F-EBC8-44A0-9B7D-9BF9EF3C88C6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:v>NlogN</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>ethanwilkes_colespencer_phw_out!$O$1:$O$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>105</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>ethanwilkes_colespencer_phw_out!$M$1:$M$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.1397940008672038E-5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.6568636235841014E-5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.159176003468815E-5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.6505149978319905E-5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.1331092497698136E-5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.6084313719900198E-5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.077528010406445E-5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.5411817415046074E-5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.9999999999999996E-5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.4544680463259522E-5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.9049825047428499E-5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6.351873642001111E-5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6.795420750050466E-5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7.2358631114164768E-5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7.6734080277505198E-5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8.1082368336569342E-5</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8.5405094908140483E-5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>8.9703681581896247E-5</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>9.3979400086720362E-5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000030-EBC8-44A0-9B7D-9BF9EF3C88C6}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -991,6 +1935,62 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Sample Size</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1038,6 +2038,7 @@
         <c:axId val="2078921232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="2.0000000000000006E-4"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1055,6 +2056,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Matri</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t>x Information</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1098,6 +2159,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -1702,16 +2794,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>457199</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>476249</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>180974</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>61912</xdr:rowOff>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2035,11 +3127,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:O20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AC12" sqref="AC12"/>
+      <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2049,9 +3141,10 @@
     <col min="5" max="6" width="4.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="2.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2076,8 +3169,28 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
+      <c r="I1">
+        <v>1</v>
+      </c>
+      <c r="J1">
+        <f>I1*0.000001</f>
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="K1">
+        <v>1E-3</v>
+      </c>
+      <c r="L1">
+        <v>1E-3</v>
+      </c>
+      <c r="M1">
+        <f>I1*LOG(I1)</f>
+        <v>0</v>
+      </c>
+      <c r="O1">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1.60403251647949E-5</v>
       </c>
@@ -2102,8 +3215,30 @@
       <c r="H2" t="s">
         <v>7</v>
       </c>
+      <c r="I2">
+        <v>2</v>
+      </c>
+      <c r="J2">
+        <f t="shared" ref="J2:J20" si="0">I2*0.000001</f>
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="K2">
+        <f>J2^2</f>
+        <v>3.9999999999999999E-12</v>
+      </c>
+      <c r="L2">
+        <f>J2^3</f>
+        <v>7.999999999999999E-18</v>
+      </c>
+      <c r="M2">
+        <f>J2*LOG(J2)*-1</f>
+        <v>1.1397940008672038E-5</v>
+      </c>
+      <c r="O2">
+        <v>15</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>3.6447048187255799E-5</v>
       </c>
@@ -2128,8 +3263,30 @@
       <c r="H3" t="s">
         <v>7</v>
       </c>
+      <c r="I3">
+        <v>3</v>
+      </c>
+      <c r="J3">
+        <f t="shared" si="0"/>
+        <v>3.0000000000000001E-6</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ref="K3:K20" si="1">J3^2</f>
+        <v>9.0000000000000012E-12</v>
+      </c>
+      <c r="L3">
+        <f t="shared" ref="L3:L20" si="2">J3^3</f>
+        <v>2.7000000000000004E-17</v>
+      </c>
+      <c r="M3">
+        <f t="shared" ref="M3:M20" si="3">J3*LOG(J3)*-1</f>
+        <v>1.6568636235841014E-5</v>
+      </c>
+      <c r="O3">
+        <v>20</v>
+      </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>6.9460391998290994E-5</v>
       </c>
@@ -2154,8 +3311,31 @@
       <c r="H4" t="s">
         <v>7</v>
       </c>
+      <c r="I4">
+        <v>4</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="0"/>
+        <v>3.9999999999999998E-6</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="1"/>
+        <v>1.6E-11</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="2"/>
+        <v>6.3999999999999992E-17</v>
+      </c>
+      <c r="M4">
+        <f t="shared" si="3"/>
+        <v>2.159176003468815E-5</v>
+      </c>
+      <c r="O4">
+        <f>O3+5</f>
+        <v>25</v>
+      </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1.20711326599121E-4</v>
       </c>
@@ -2180,8 +3360,31 @@
       <c r="H5" t="s">
         <v>7</v>
       </c>
+      <c r="I5">
+        <v>5</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="0"/>
+        <v>4.9999999999999996E-6</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="1"/>
+        <v>2.4999999999999994E-11</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="2"/>
+        <v>1.2499999999999996E-16</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="3"/>
+        <v>2.6505149978319905E-5</v>
+      </c>
+      <c r="O5">
+        <f t="shared" ref="O5:O20" si="4">O4+5</f>
+        <v>30</v>
+      </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1.78500652313232E-4</v>
       </c>
@@ -2206,8 +3409,31 @@
       <c r="H6" t="s">
         <v>7</v>
       </c>
+      <c r="I6">
+        <v>6</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="0"/>
+        <v>6.0000000000000002E-6</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="1"/>
+        <v>3.6000000000000005E-11</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="2"/>
+        <v>2.1600000000000003E-16</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="3"/>
+        <v>3.1331092497698136E-5</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="4"/>
+        <v>35</v>
+      </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2.7098274230957E-4</v>
       </c>
@@ -2232,8 +3458,31 @@
       <c r="H7" t="s">
         <v>7</v>
       </c>
+      <c r="I7">
+        <v>7</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="0"/>
+        <v>6.9999999999999999E-6</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="1"/>
+        <v>4.8999999999999999E-11</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="2"/>
+        <v>3.43E-16</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="3"/>
+        <v>3.6084313719900198E-5</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="4"/>
+        <v>40</v>
+      </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>3.8077878952026299E-4</v>
       </c>
@@ -2258,8 +3507,31 @@
       <c r="H8" t="s">
         <v>7</v>
       </c>
+      <c r="I8">
+        <v>8</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="0"/>
+        <v>7.9999999999999996E-6</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="1"/>
+        <v>6.3999999999999999E-11</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="2"/>
+        <v>5.1199999999999994E-16</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="3"/>
+        <v>4.077528010406445E-5</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="4"/>
+        <v>45</v>
+      </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5.3909730911254805E-4</v>
       </c>
@@ -2284,8 +3556,31 @@
       <c r="H9" t="s">
         <v>7</v>
       </c>
+      <c r="I9">
+        <v>9</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="0"/>
+        <v>9.0000000000000002E-6</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="1"/>
+        <v>8.1000000000000005E-11</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="2"/>
+        <v>7.2900000000000001E-16</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="3"/>
+        <v>4.5411817415046074E-5</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="4"/>
+        <v>50</v>
+      </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>7.3981046676635704E-4</v>
       </c>
@@ -2310,8 +3605,31 @@
       <c r="H10" t="s">
         <v>7</v>
       </c>
+      <c r="I10">
+        <v>10</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="0"/>
+        <v>9.9999999999999991E-6</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="1"/>
+        <v>9.9999999999999978E-11</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="2"/>
+        <v>9.9999999999999968E-16</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="3"/>
+        <v>4.9999999999999996E-5</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="4"/>
+        <v>55</v>
+      </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9.3150806427001905E-4</v>
       </c>
@@ -2336,8 +3654,31 @@
       <c r="H11" t="s">
         <v>7</v>
       </c>
+      <c r="I11">
+        <v>11</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="0"/>
+        <v>1.1E-5</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="1"/>
+        <v>1.21E-10</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="2"/>
+        <v>1.3309999999999999E-15</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="3"/>
+        <v>5.4544680463259522E-5</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="4"/>
+        <v>60</v>
+      </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1.17854833602905E-3</v>
       </c>
@@ -2362,8 +3703,31 @@
       <c r="H12" t="s">
         <v>7</v>
       </c>
+      <c r="I12">
+        <v>12</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="0"/>
+        <v>1.2E-5</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="1"/>
+        <v>1.4400000000000002E-10</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="2"/>
+        <v>1.7280000000000003E-15</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="3"/>
+        <v>5.9049825047428499E-5</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="4"/>
+        <v>65</v>
+      </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1.45844602584838E-3</v>
       </c>
@@ -2388,8 +3752,31 @@
       <c r="H13" t="s">
         <v>7</v>
       </c>
+      <c r="I13">
+        <v>13</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="0"/>
+        <v>1.2999999999999999E-5</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="1"/>
+        <v>1.6899999999999999E-10</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="2"/>
+        <v>2.1969999999999996E-15</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="3"/>
+        <v>6.351873642001111E-5</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="4"/>
+        <v>70</v>
+      </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1.71746635437011E-3</v>
       </c>
@@ -2414,8 +3801,31 @@
       <c r="H14" t="s">
         <v>7</v>
       </c>
+      <c r="I14">
+        <v>14</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="0"/>
+        <v>1.4E-5</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="1"/>
+        <v>1.96E-10</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="2"/>
+        <v>2.744E-15</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="3"/>
+        <v>6.795420750050466E-5</v>
+      </c>
+      <c r="O14">
+        <f t="shared" si="4"/>
+        <v>75</v>
+      </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2.13365173339843E-3</v>
       </c>
@@ -2440,8 +3850,31 @@
       <c r="H15" t="s">
         <v>7</v>
       </c>
+      <c r="I15">
+        <v>15</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="0"/>
+        <v>1.4999999999999999E-5</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="1"/>
+        <v>2.2499999999999997E-10</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="2"/>
+        <v>3.3749999999999994E-15</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="3"/>
+        <v>7.2358631114164768E-5</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="4"/>
+        <v>80</v>
+      </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2.6068348884582498E-3</v>
       </c>
@@ -2466,8 +3899,31 @@
       <c r="H16" t="s">
         <v>7</v>
       </c>
+      <c r="I16">
+        <v>16</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="0"/>
+        <v>1.5999999999999999E-5</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="1"/>
+        <v>2.5599999999999999E-10</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="2"/>
+        <v>4.0959999999999995E-15</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="3"/>
+        <v>7.6734080277505198E-5</v>
+      </c>
+      <c r="O16">
+        <f t="shared" si="4"/>
+        <v>85</v>
+      </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>3.0079078674316402E-3</v>
       </c>
@@ -2492,8 +3948,31 @@
       <c r="H17" t="s">
         <v>7</v>
       </c>
+      <c r="I17">
+        <v>17</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="0"/>
+        <v>1.7E-5</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="1"/>
+        <v>2.8899999999999998E-10</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="2"/>
+        <v>4.913E-15</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="3"/>
+        <v>8.1082368336569342E-5</v>
+      </c>
+      <c r="O17">
+        <f t="shared" si="4"/>
+        <v>90</v>
+      </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>3.49193525314331E-3</v>
       </c>
@@ -2518,8 +3997,31 @@
       <c r="H18" t="s">
         <v>7</v>
       </c>
+      <c r="I18">
+        <v>18</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="0"/>
+        <v>1.8E-5</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="1"/>
+        <v>3.2400000000000002E-10</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="2"/>
+        <v>5.8320000000000001E-15</v>
+      </c>
+      <c r="M18">
+        <f t="shared" si="3"/>
+        <v>8.5405094908140483E-5</v>
+      </c>
+      <c r="O18">
+        <f t="shared" si="4"/>
+        <v>95</v>
+      </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>4.1812381744384701E-3</v>
       </c>
@@ -2544,8 +4046,31 @@
       <c r="H19" t="s">
         <v>7</v>
       </c>
+      <c r="I19">
+        <v>19</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="0"/>
+        <v>1.8999999999999998E-5</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="1"/>
+        <v>3.6099999999999989E-10</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="2"/>
+        <v>6.8589999999999973E-15</v>
+      </c>
+      <c r="M19">
+        <f t="shared" si="3"/>
+        <v>8.9703681581896247E-5</v>
+      </c>
+      <c r="O19">
+        <f t="shared" si="4"/>
+        <v>100</v>
+      </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>5.1559929847717198E-3</v>
       </c>
@@ -2569,6 +4094,29 @@
       </c>
       <c r="H20" t="s">
         <v>7</v>
+      </c>
+      <c r="I20">
+        <v>20</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="0"/>
+        <v>1.9999999999999998E-5</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="1"/>
+        <v>3.9999999999999991E-10</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="2"/>
+        <v>7.9999999999999975E-15</v>
+      </c>
+      <c r="M20">
+        <f t="shared" si="3"/>
+        <v>9.3979400086720362E-5</v>
+      </c>
+      <c r="O20">
+        <f t="shared" si="4"/>
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>